<commit_message>
llm now takes inspiration from the dict instead of relying on it
</commit_message>
<xml_diff>
--- a/data/sample_transactions_truth.xlsx
+++ b/data/sample_transactions_truth.xlsx
@@ -217,12 +217,12 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="K41" activeCellId="0" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>